<commit_message>
Cambio correlativo por eliminacion de un CE
</commit_message>
<xml_diff>
--- a/puntos_ce.xlsx
+++ b/puntos_ce.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="578">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -1197,12 +1197,6 @@
   </si>
   <si>
     <t xml:space="preserve">No recibe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CENTRO ESCOLAR COLONIA QUIÑONEZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALLE PRINCIPAL, PASAJE LA LABOR, COLONIA QUIÑONEZ</t>
   </si>
   <si>
     <t xml:space="preserve">CENTRO ESCOLAR COLONIA SANTA LUCIA</t>
@@ -1895,7 +1889,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1941,19 +1935,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2033,16 +2015,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M192"/>
+  <dimension ref="A1:M191"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I169" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L205" activeCellId="0" sqref="L205"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A191" activeCellId="0" sqref="A191"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="4" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="114.43"/>
@@ -6771,7 +6753,7 @@
       <c r="A116" s="10" t="n">
         <v>118</v>
       </c>
-      <c r="B116" s="11" t="s">
+      <c r="B116" s="10" t="s">
         <v>386</v>
       </c>
       <c r="C116" s="10"/>
@@ -6787,10 +6769,10 @@
       <c r="G116" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H116" s="11" t="s">
+      <c r="H116" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="I116" s="12" t="n">
+      <c r="I116" s="3" t="n">
         <v>29</v>
       </c>
       <c r="J116" s="10" t="s">
@@ -6799,10 +6781,10 @@
       <c r="K116" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L116" s="13" t="n">
+      <c r="L116" s="11" t="n">
         <v>-89.212615</v>
       </c>
-      <c r="M116" s="12" t="n">
+      <c r="M116" s="3" t="n">
         <v>13.713098</v>
       </c>
     </row>
@@ -6810,7 +6792,7 @@
       <c r="A117" s="10" t="n">
         <v>119</v>
       </c>
-      <c r="B117" s="11" t="s">
+      <c r="B117" s="10" t="s">
         <v>389</v>
       </c>
       <c r="C117" s="10"/>
@@ -6826,10 +6808,10 @@
       <c r="G117" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H117" s="11" t="s">
+      <c r="H117" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="I117" s="12" t="n">
+      <c r="I117" s="3" t="n">
         <v>12</v>
       </c>
       <c r="J117" s="10" t="s">
@@ -6838,18 +6820,18 @@
       <c r="K117" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L117" s="12" t="n">
+      <c r="L117" s="3" t="n">
         <v>-89.181177</v>
       </c>
-      <c r="M117" s="12" t="n">
+      <c r="M117" s="3" t="n">
         <v>13.713382</v>
       </c>
     </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="n">
         <v>120</v>
       </c>
-      <c r="B118" s="11" t="s">
+      <c r="B118" s="10" t="s">
         <v>392</v>
       </c>
       <c r="C118" s="10"/>
@@ -6865,11 +6847,11 @@
       <c r="G118" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H118" s="11" t="s">
+      <c r="H118" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="I118" s="12" t="n">
-        <v>0</v>
+      <c r="I118" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="J118" s="10" t="s">
         <v>391</v>
@@ -6877,18 +6859,18 @@
       <c r="K118" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L118" s="12" t="n">
-        <v>-89.566933</v>
-      </c>
-      <c r="M118" s="12" t="n">
-        <v>13.992794</v>
+      <c r="L118" s="11" t="n">
+        <v>-89.221619</v>
+      </c>
+      <c r="M118" s="3" t="n">
+        <v>13.70812</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="n">
         <v>121</v>
       </c>
-      <c r="B119" s="11" t="s">
+      <c r="B119" s="10" t="s">
         <v>394</v>
       </c>
       <c r="C119" s="10"/>
@@ -6904,31 +6886,31 @@
       <c r="G119" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H119" s="11" t="s">
+      <c r="H119" s="10" t="s">
         <v>395</v>
       </c>
-      <c r="I119" s="12" t="n">
-        <v>8</v>
+      <c r="I119" s="3" t="n">
+        <v>27</v>
       </c>
       <c r="J119" s="10" t="s">
-        <v>391</v>
+        <v>181</v>
       </c>
       <c r="K119" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L119" s="13" t="n">
-        <v>-89.221619</v>
-      </c>
-      <c r="M119" s="12" t="n">
-        <v>13.70812</v>
+        <v>396</v>
+      </c>
+      <c r="L119" s="11" t="n">
+        <v>-89.212305</v>
+      </c>
+      <c r="M119" s="3" t="n">
+        <v>13.699409</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="n">
         <v>122</v>
       </c>
-      <c r="B120" s="11" t="s">
-        <v>396</v>
+      <c r="B120" s="10" t="s">
+        <v>397</v>
       </c>
       <c r="C120" s="10"/>
       <c r="D120" s="3" t="s">
@@ -6943,33 +6925,33 @@
       <c r="G120" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H120" s="11" t="s">
-        <v>397</v>
-      </c>
-      <c r="I120" s="12" t="n">
-        <v>27</v>
+      <c r="H120" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="I120" s="3" t="n">
+        <v>6</v>
       </c>
       <c r="J120" s="10" t="s">
-        <v>181</v>
+        <v>391</v>
       </c>
       <c r="K120" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="L120" s="13" t="n">
-        <v>-89.212305</v>
-      </c>
-      <c r="M120" s="12" t="n">
-        <v>13.699409</v>
+        <v>20</v>
+      </c>
+      <c r="L120" s="11" t="n">
+        <v>-89.180931</v>
+      </c>
+      <c r="M120" s="3" t="n">
+        <v>13.707918</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="10" t="n">
+      <c r="A121" s="3" t="n">
         <v>123</v>
       </c>
-      <c r="B121" s="11" t="s">
+      <c r="B121" s="10" t="s">
         <v>399</v>
       </c>
-      <c r="C121" s="10"/>
+      <c r="C121" s="3"/>
       <c r="D121" s="3" t="s">
         <v>387</v>
       </c>
@@ -6982,33 +6964,33 @@
       <c r="G121" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H121" s="11" t="s">
+      <c r="H121" s="10" t="s">
         <v>400</v>
       </c>
-      <c r="I121" s="12" t="n">
-        <v>6</v>
-      </c>
-      <c r="J121" s="10" t="s">
+      <c r="I121" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="J121" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K121" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L121" s="13" t="n">
-        <v>-89.180931</v>
-      </c>
-      <c r="M121" s="12" t="n">
-        <v>13.707918</v>
+        <v>401</v>
+      </c>
+      <c r="L121" s="11" t="n">
+        <v>-89.212703</v>
+      </c>
+      <c r="M121" s="3" t="n">
+        <v>13.693706</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="12" t="n">
+      <c r="A122" s="3" t="n">
         <v>124</v>
       </c>
-      <c r="B122" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="C122" s="12"/>
+      <c r="B122" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="C122" s="3"/>
       <c r="D122" s="3" t="s">
         <v>387</v>
       </c>
@@ -7021,33 +7003,33 @@
       <c r="G122" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H122" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="I122" s="12" t="n">
-        <v>30</v>
-      </c>
-      <c r="J122" s="12" t="s">
+      <c r="H122" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="I122" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="J122" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K122" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="L122" s="13" t="n">
-        <v>-89.212703</v>
-      </c>
-      <c r="M122" s="12" t="n">
-        <v>13.693706</v>
+        <v>404</v>
+      </c>
+      <c r="L122" s="11" t="n">
+        <v>-89.211608</v>
+      </c>
+      <c r="M122" s="3" t="n">
+        <v>13.72273</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="12" t="n">
+      <c r="A123" s="3" t="n">
         <v>125</v>
       </c>
-      <c r="B123" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="C123" s="12"/>
+      <c r="B123" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="C123" s="3"/>
       <c r="D123" s="3" t="s">
         <v>387</v>
       </c>
@@ -7060,33 +7042,33 @@
       <c r="G123" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H123" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="I123" s="12" t="n">
-        <v>41</v>
-      </c>
-      <c r="J123" s="12" t="s">
+      <c r="H123" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="I123" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J123" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K123" s="3" t="s">
-        <v>406</v>
-      </c>
-      <c r="L123" s="13" t="n">
-        <v>-89.211608</v>
-      </c>
-      <c r="M123" s="12" t="n">
-        <v>13.72273</v>
+        <v>20</v>
+      </c>
+      <c r="L123" s="11" t="n">
+        <v>-89.201527</v>
+      </c>
+      <c r="M123" s="3" t="n">
+        <v>13.690578</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="12" t="n">
+      <c r="A124" s="3" t="n">
         <v>126</v>
       </c>
-      <c r="B124" s="11" t="s">
+      <c r="B124" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="C124" s="12"/>
+      <c r="C124" s="3"/>
       <c r="D124" s="3" t="s">
         <v>387</v>
       </c>
@@ -7099,33 +7081,33 @@
       <c r="G124" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H124" s="11" t="s">
+      <c r="H124" s="10" t="s">
         <v>408</v>
       </c>
-      <c r="I124" s="12" t="n">
-        <v>7</v>
-      </c>
-      <c r="J124" s="12" t="s">
+      <c r="I124" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="J124" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K124" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L124" s="13" t="n">
-        <v>-89.201527</v>
-      </c>
-      <c r="M124" s="12" t="n">
-        <v>13.690578</v>
+        <v>409</v>
+      </c>
+      <c r="L124" s="7" t="n">
+        <v>-89.209158</v>
+      </c>
+      <c r="M124" s="3" t="n">
+        <v>13.689075</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="12" t="n">
+      <c r="A125" s="3" t="n">
         <v>127</v>
       </c>
-      <c r="B125" s="11" t="s">
-        <v>409</v>
-      </c>
-      <c r="C125" s="12"/>
+      <c r="B125" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="C125" s="3"/>
       <c r="D125" s="3" t="s">
         <v>387</v>
       </c>
@@ -7138,33 +7120,33 @@
       <c r="G125" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H125" s="11" t="s">
-        <v>410</v>
-      </c>
-      <c r="I125" s="12" t="n">
-        <v>6</v>
-      </c>
-      <c r="J125" s="12" t="s">
+      <c r="H125" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="I125" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="J125" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K125" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="L125" s="14" t="n">
-        <v>-89.209158</v>
-      </c>
-      <c r="M125" s="12" t="n">
-        <v>13.689075</v>
+        <v>412</v>
+      </c>
+      <c r="L125" s="7" t="n">
+        <v>-89.194719</v>
+      </c>
+      <c r="M125" s="3" t="n">
+        <v>13.71282</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="12" t="n">
+      <c r="A126" s="3" t="n">
         <v>128</v>
       </c>
-      <c r="B126" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="C126" s="12"/>
+      <c r="B126" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="C126" s="3"/>
       <c r="D126" s="3" t="s">
         <v>387</v>
       </c>
@@ -7177,33 +7159,33 @@
       <c r="G126" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H126" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="I126" s="12" t="n">
-        <v>39</v>
-      </c>
-      <c r="J126" s="12" t="s">
-        <v>391</v>
+      <c r="H126" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="I126" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="J126" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="K126" s="3" t="s">
-        <v>414</v>
-      </c>
-      <c r="L126" s="14" t="n">
-        <v>-89.194719</v>
-      </c>
-      <c r="M126" s="12" t="n">
-        <v>13.71282</v>
+        <v>20</v>
+      </c>
+      <c r="L126" s="7" t="n">
+        <v>-89.182013</v>
+      </c>
+      <c r="M126" s="3" t="n">
+        <v>13.694149</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="12" t="n">
+      <c r="A127" s="3" t="n">
         <v>129</v>
       </c>
-      <c r="B127" s="11" t="s">
+      <c r="B127" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="C127" s="12"/>
+      <c r="C127" s="3"/>
       <c r="D127" s="3" t="s">
         <v>387</v>
       </c>
@@ -7216,33 +7198,33 @@
       <c r="G127" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H127" s="11" t="s">
+      <c r="H127" s="10" t="s">
         <v>416</v>
       </c>
-      <c r="I127" s="12" t="n">
-        <v>30</v>
-      </c>
-      <c r="J127" s="12" t="s">
-        <v>132</v>
+      <c r="I127" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="J127" s="3" t="s">
+        <v>417</v>
       </c>
       <c r="K127" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L127" s="14" t="n">
-        <v>-89.182013</v>
-      </c>
-      <c r="M127" s="12" t="n">
-        <v>13.694149</v>
+        <v>418</v>
+      </c>
+      <c r="L127" s="7" t="n">
+        <v>-89.190272</v>
+      </c>
+      <c r="M127" s="3" t="n">
+        <v>13.687554</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="12" t="n">
+      <c r="A128" s="3" t="n">
         <v>130</v>
       </c>
-      <c r="B128" s="11" t="s">
-        <v>417</v>
-      </c>
-      <c r="C128" s="12"/>
+      <c r="B128" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="C128" s="3"/>
       <c r="D128" s="3" t="s">
         <v>387</v>
       </c>
@@ -7255,33 +7237,33 @@
       <c r="G128" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H128" s="11" t="s">
-        <v>418</v>
-      </c>
-      <c r="I128" s="12" t="n">
-        <v>86</v>
-      </c>
-      <c r="J128" s="12" t="s">
-        <v>419</v>
+      <c r="H128" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="I128" s="3" t="n">
+        <v>364</v>
+      </c>
+      <c r="J128" s="3" t="s">
+        <v>421</v>
       </c>
       <c r="K128" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="L128" s="14" t="n">
-        <v>-89.190272</v>
-      </c>
-      <c r="M128" s="12" t="n">
-        <v>13.687554</v>
+        <v>20</v>
+      </c>
+      <c r="L128" s="7" t="n">
+        <v>-89.191616</v>
+      </c>
+      <c r="M128" s="3" t="n">
+        <v>13.701683</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="12" t="n">
+      <c r="A129" s="3" t="n">
         <v>131</v>
       </c>
-      <c r="B129" s="11" t="s">
-        <v>421</v>
-      </c>
-      <c r="C129" s="12"/>
+      <c r="B129" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="C129" s="3"/>
       <c r="D129" s="3" t="s">
         <v>387</v>
       </c>
@@ -7294,33 +7276,33 @@
       <c r="G129" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H129" s="11" t="s">
-        <v>422</v>
-      </c>
-      <c r="I129" s="12" t="n">
-        <v>364</v>
-      </c>
-      <c r="J129" s="12" t="s">
+      <c r="H129" s="10" t="s">
         <v>423</v>
       </c>
+      <c r="I129" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J129" s="3" t="s">
+        <v>391</v>
+      </c>
       <c r="K129" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L129" s="14" t="n">
-        <v>-89.191616</v>
-      </c>
-      <c r="M129" s="12" t="n">
-        <v>13.701683</v>
+        <v>424</v>
+      </c>
+      <c r="L129" s="7" t="n">
+        <v>-89.181825</v>
+      </c>
+      <c r="M129" s="3" t="n">
+        <v>13.713051</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="12" t="n">
+      <c r="A130" s="3" t="n">
         <v>132</v>
       </c>
-      <c r="B130" s="11" t="s">
-        <v>424</v>
-      </c>
-      <c r="C130" s="12"/>
+      <c r="B130" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="C130" s="3"/>
       <c r="D130" s="3" t="s">
         <v>387</v>
       </c>
@@ -7333,33 +7315,33 @@
       <c r="G130" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H130" s="11" t="s">
-        <v>425</v>
-      </c>
-      <c r="I130" s="12" t="n">
-        <v>3</v>
-      </c>
-      <c r="J130" s="12" t="s">
+      <c r="H130" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="I130" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="J130" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K130" s="3" t="s">
-        <v>426</v>
-      </c>
-      <c r="L130" s="14" t="n">
-        <v>-89.181825</v>
-      </c>
-      <c r="M130" s="12" t="n">
-        <v>13.713051</v>
+        <v>20</v>
+      </c>
+      <c r="L130" s="7" t="n">
+        <v>-89.183451</v>
+      </c>
+      <c r="M130" s="3" t="n">
+        <v>13.70036</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="12" t="n">
+      <c r="A131" s="3" t="n">
         <v>133</v>
       </c>
-      <c r="B131" s="11" t="s">
+      <c r="B131" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="C131" s="12"/>
+      <c r="C131" s="3"/>
       <c r="D131" s="3" t="s">
         <v>387</v>
       </c>
@@ -7372,33 +7354,33 @@
       <c r="G131" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H131" s="11" t="s">
+      <c r="H131" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="I131" s="12" t="n">
-        <v>19</v>
-      </c>
-      <c r="J131" s="12" t="s">
-        <v>391</v>
+      <c r="I131" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="J131" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="K131" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L131" s="14" t="n">
-        <v>-89.183451</v>
-      </c>
-      <c r="M131" s="12" t="n">
-        <v>13.70036</v>
+        <v>429</v>
+      </c>
+      <c r="L131" s="7" t="n">
+        <v>-89.206068</v>
+      </c>
+      <c r="M131" s="3" t="n">
+        <v>13.71547</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="12" t="n">
+      <c r="A132" s="3" t="n">
         <v>134</v>
       </c>
-      <c r="B132" s="11" t="s">
-        <v>429</v>
-      </c>
-      <c r="C132" s="12"/>
+      <c r="B132" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="C132" s="3"/>
       <c r="D132" s="3" t="s">
         <v>387</v>
       </c>
@@ -7411,33 +7393,33 @@
       <c r="G132" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H132" s="11" t="s">
-        <v>430</v>
-      </c>
-      <c r="I132" s="12" t="n">
-        <v>25</v>
-      </c>
-      <c r="J132" s="12" t="s">
-        <v>181</v>
+      <c r="H132" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="I132" s="3" t="n">
+        <v>101</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>417</v>
       </c>
       <c r="K132" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="L132" s="14" t="n">
-        <v>-89.206068</v>
-      </c>
-      <c r="M132" s="12" t="n">
-        <v>13.71547</v>
+        <v>432</v>
+      </c>
+      <c r="L132" s="7" t="n">
+        <v>-89.195427</v>
+      </c>
+      <c r="M132" s="3" t="n">
+        <v>13.68631</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="12" t="n">
+      <c r="A133" s="3" t="n">
         <v>135</v>
       </c>
-      <c r="B133" s="11" t="s">
-        <v>432</v>
-      </c>
-      <c r="C133" s="12"/>
+      <c r="B133" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="C133" s="3"/>
       <c r="D133" s="3" t="s">
         <v>387</v>
       </c>
@@ -7450,33 +7432,33 @@
       <c r="G133" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H133" s="11" t="s">
-        <v>433</v>
-      </c>
-      <c r="I133" s="12" t="n">
-        <v>101</v>
-      </c>
-      <c r="J133" s="12" t="s">
-        <v>419</v>
+      <c r="H133" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="I133" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>435</v>
       </c>
       <c r="K133" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="L133" s="14" t="n">
-        <v>-89.195427</v>
-      </c>
-      <c r="M133" s="12" t="n">
-        <v>13.68631</v>
+        <v>20</v>
+      </c>
+      <c r="L133" s="7" t="n">
+        <v>-89.179054</v>
+      </c>
+      <c r="M133" s="3" t="n">
+        <v>13.695622</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="12" t="n">
+      <c r="A134" s="3" t="n">
         <v>136</v>
       </c>
-      <c r="B134" s="11" t="s">
-        <v>435</v>
-      </c>
-      <c r="C134" s="12"/>
+      <c r="B134" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="C134" s="3"/>
       <c r="D134" s="3" t="s">
         <v>387</v>
       </c>
@@ -7489,33 +7471,33 @@
       <c r="G134" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H134" s="11" t="s">
-        <v>436</v>
-      </c>
-      <c r="I134" s="12" t="n">
-        <v>35</v>
-      </c>
-      <c r="J134" s="12" t="s">
+      <c r="H134" s="10" t="s">
         <v>437</v>
       </c>
+      <c r="I134" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="K134" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L134" s="14" t="n">
-        <v>-89.179054</v>
-      </c>
-      <c r="M134" s="12" t="n">
-        <v>13.695622</v>
+        <v>438</v>
+      </c>
+      <c r="L134" s="7" t="n">
+        <v>-89.192777</v>
+      </c>
+      <c r="M134" s="3" t="n">
+        <v>13.691182</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="12" t="n">
+      <c r="A135" s="3" t="n">
         <v>137</v>
       </c>
-      <c r="B135" s="11" t="s">
-        <v>438</v>
-      </c>
-      <c r="C135" s="12"/>
+      <c r="B135" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="C135" s="3"/>
       <c r="D135" s="3" t="s">
         <v>387</v>
       </c>
@@ -7528,33 +7510,33 @@
       <c r="G135" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H135" s="11" t="s">
-        <v>439</v>
-      </c>
-      <c r="I135" s="12" t="n">
-        <v>32</v>
-      </c>
-      <c r="J135" s="12" t="s">
-        <v>181</v>
+      <c r="H135" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="I135" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="J135" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="K135" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="L135" s="14" t="n">
-        <v>-89.192777</v>
-      </c>
-      <c r="M135" s="12" t="n">
-        <v>13.691182</v>
+        <v>441</v>
+      </c>
+      <c r="L135" s="7" t="n">
+        <v>-89.191278</v>
+      </c>
+      <c r="M135" s="3" t="n">
+        <v>13.681215</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="12" t="n">
+      <c r="A136" s="3" t="n">
         <v>138</v>
       </c>
-      <c r="B136" s="11" t="s">
-        <v>441</v>
-      </c>
-      <c r="C136" s="12"/>
+      <c r="B136" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="C136" s="3"/>
       <c r="D136" s="3" t="s">
         <v>387</v>
       </c>
@@ -7567,33 +7549,33 @@
       <c r="G136" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H136" s="11" t="s">
-        <v>442</v>
-      </c>
-      <c r="I136" s="12" t="n">
-        <v>38</v>
-      </c>
-      <c r="J136" s="12" t="s">
+      <c r="H136" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="I136" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="J136" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K136" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="L136" s="14" t="n">
-        <v>-89.191278</v>
-      </c>
-      <c r="M136" s="12" t="n">
-        <v>13.681215</v>
+        <v>20</v>
+      </c>
+      <c r="L136" s="7" t="n">
+        <v>-89.188601</v>
+      </c>
+      <c r="M136" s="3" t="n">
+        <v>13.696283</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="12" t="n">
+      <c r="A137" s="3" t="n">
         <v>139</v>
       </c>
-      <c r="B137" s="11" t="s">
+      <c r="B137" s="10" t="s">
         <v>444</v>
       </c>
-      <c r="C137" s="12"/>
+      <c r="C137" s="3"/>
       <c r="D137" s="3" t="s">
         <v>387</v>
       </c>
@@ -7606,33 +7588,33 @@
       <c r="G137" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H137" s="11" t="s">
+      <c r="H137" s="10" t="s">
         <v>445</v>
       </c>
-      <c r="I137" s="12" t="n">
-        <v>27</v>
-      </c>
-      <c r="J137" s="12" t="s">
+      <c r="I137" s="3" t="n">
+        <v>175</v>
+      </c>
+      <c r="J137" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K137" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L137" s="14" t="n">
-        <v>-89.188601</v>
-      </c>
-      <c r="M137" s="12" t="n">
-        <v>13.696283</v>
+        <v>446</v>
+      </c>
+      <c r="L137" s="7" t="n">
+        <v>-89.24847</v>
+      </c>
+      <c r="M137" s="3" t="n">
+        <v>13.70499</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="12" t="n">
+      <c r="A138" s="3" t="n">
         <v>140</v>
       </c>
-      <c r="B138" s="11" t="s">
-        <v>446</v>
-      </c>
-      <c r="C138" s="12"/>
+      <c r="B138" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="C138" s="3"/>
       <c r="D138" s="3" t="s">
         <v>387</v>
       </c>
@@ -7645,33 +7627,33 @@
       <c r="G138" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H138" s="11" t="s">
-        <v>447</v>
-      </c>
-      <c r="I138" s="12" t="n">
-        <v>175</v>
-      </c>
-      <c r="J138" s="12" t="s">
+      <c r="H138" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="I138" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="J138" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K138" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="L138" s="14" t="n">
-        <v>-89.24847</v>
-      </c>
-      <c r="M138" s="12" t="n">
-        <v>13.70499</v>
+        <v>449</v>
+      </c>
+      <c r="L138" s="7" t="n">
+        <v>-89.193241</v>
+      </c>
+      <c r="M138" s="3" t="n">
+        <v>13.692764</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="12" t="n">
+      <c r="A139" s="3" t="n">
         <v>141</v>
       </c>
-      <c r="B139" s="11" t="s">
-        <v>449</v>
-      </c>
-      <c r="C139" s="12"/>
+      <c r="B139" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="C139" s="3"/>
       <c r="D139" s="3" t="s">
         <v>387</v>
       </c>
@@ -7684,33 +7666,33 @@
       <c r="G139" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H139" s="11" t="s">
-        <v>450</v>
-      </c>
-      <c r="I139" s="12" t="n">
-        <v>55</v>
-      </c>
-      <c r="J139" s="12" t="s">
-        <v>391</v>
+      <c r="H139" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="I139" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="J139" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="K139" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="L139" s="14" t="n">
-        <v>-89.193241</v>
-      </c>
-      <c r="M139" s="12" t="n">
-        <v>13.692764</v>
+        <v>20</v>
+      </c>
+      <c r="L139" s="7" t="n">
+        <v>-89.214717</v>
+      </c>
+      <c r="M139" s="3" t="n">
+        <v>13.682848</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="12" t="n">
+      <c r="A140" s="3" t="n">
         <v>142</v>
       </c>
-      <c r="B140" s="11" t="s">
+      <c r="B140" s="10" t="s">
         <v>452</v>
       </c>
-      <c r="C140" s="12"/>
+      <c r="C140" s="3"/>
       <c r="D140" s="3" t="s">
         <v>387</v>
       </c>
@@ -7723,33 +7705,33 @@
       <c r="G140" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H140" s="11" t="s">
+      <c r="H140" s="10" t="s">
         <v>453</v>
       </c>
-      <c r="I140" s="12" t="n">
-        <v>22</v>
-      </c>
-      <c r="J140" s="12" t="s">
-        <v>181</v>
+      <c r="I140" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J140" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="K140" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L140" s="14" t="n">
-        <v>-89.214717</v>
-      </c>
-      <c r="M140" s="12" t="n">
-        <v>13.682848</v>
+        <v>454</v>
+      </c>
+      <c r="L140" s="7" t="n">
+        <v>-89.177821</v>
+      </c>
+      <c r="M140" s="3" t="n">
+        <v>13.705559</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="12" t="n">
+      <c r="A141" s="3" t="n">
         <v>143</v>
       </c>
-      <c r="B141" s="11" t="s">
-        <v>454</v>
-      </c>
-      <c r="C141" s="12"/>
+      <c r="B141" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="C141" s="3"/>
       <c r="D141" s="3" t="s">
         <v>387</v>
       </c>
@@ -7762,33 +7744,33 @@
       <c r="G141" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H141" s="11" t="s">
-        <v>455</v>
-      </c>
-      <c r="I141" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J141" s="12" t="s">
-        <v>391</v>
+      <c r="H141" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="I141" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="J141" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="K141" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="L141" s="14" t="n">
-        <v>-89.177821</v>
-      </c>
-      <c r="M141" s="12" t="n">
-        <v>13.705559</v>
+        <v>457</v>
+      </c>
+      <c r="L141" s="7" t="n">
+        <v>-89.237565</v>
+      </c>
+      <c r="M141" s="3" t="n">
+        <v>13.705584</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="12" t="n">
+      <c r="A142" s="3" t="n">
         <v>144</v>
       </c>
-      <c r="B142" s="11" t="s">
-        <v>457</v>
-      </c>
-      <c r="C142" s="12"/>
+      <c r="B142" s="10" t="s">
+        <v>458</v>
+      </c>
+      <c r="C142" s="3"/>
       <c r="D142" s="3" t="s">
         <v>387</v>
       </c>
@@ -7801,33 +7783,33 @@
       <c r="G142" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H142" s="11" t="s">
-        <v>458</v>
-      </c>
-      <c r="I142" s="12" t="n">
-        <v>61</v>
-      </c>
-      <c r="J142" s="12" t="s">
-        <v>132</v>
+      <c r="H142" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="I142" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="J142" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="K142" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="L142" s="14" t="n">
-        <v>-89.237565</v>
-      </c>
-      <c r="M142" s="12" t="n">
-        <v>13.705584</v>
+        <v>460</v>
+      </c>
+      <c r="L142" s="7" t="n">
+        <v>-89.181126</v>
+      </c>
+      <c r="M142" s="3" t="n">
+        <v>13.718242</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="12" t="n">
+      <c r="A143" s="3" t="n">
         <v>145</v>
       </c>
-      <c r="B143" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="C143" s="12"/>
+      <c r="B143" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C143" s="3"/>
       <c r="D143" s="3" t="s">
         <v>387</v>
       </c>
@@ -7840,33 +7822,33 @@
       <c r="G143" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H143" s="11" t="s">
-        <v>461</v>
-      </c>
-      <c r="I143" s="12" t="n">
-        <v>22</v>
-      </c>
-      <c r="J143" s="12" t="s">
-        <v>391</v>
+      <c r="H143" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="I143" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="J143" s="3" t="s">
+        <v>417</v>
       </c>
       <c r="K143" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="L143" s="14" t="n">
-        <v>-89.181126</v>
-      </c>
-      <c r="M143" s="12" t="n">
-        <v>13.718242</v>
+        <v>20</v>
+      </c>
+      <c r="L143" s="7" t="n">
+        <v>-89.192498</v>
+      </c>
+      <c r="M143" s="3" t="n">
+        <v>13.702109</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="12" t="n">
+      <c r="A144" s="3" t="n">
         <v>146</v>
       </c>
-      <c r="B144" s="11" t="s">
+      <c r="B144" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="C144" s="12"/>
+      <c r="C144" s="3"/>
       <c r="D144" s="3" t="s">
         <v>387</v>
       </c>
@@ -7879,33 +7861,33 @@
       <c r="G144" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H144" s="11" t="s">
+      <c r="H144" s="10" t="s">
         <v>464</v>
       </c>
-      <c r="I144" s="12" t="n">
-        <v>21</v>
-      </c>
-      <c r="J144" s="12" t="s">
-        <v>419</v>
+      <c r="I144" s="3" t="n">
+        <v>172</v>
+      </c>
+      <c r="J144" s="3" t="s">
+        <v>435</v>
       </c>
       <c r="K144" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L144" s="14" t="n">
-        <v>-89.192498</v>
-      </c>
-      <c r="M144" s="12" t="n">
-        <v>13.702109</v>
+        <v>465</v>
+      </c>
+      <c r="L144" s="7" t="n">
+        <v>-89.193359</v>
+      </c>
+      <c r="M144" s="3" t="n">
+        <v>13.685799</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="12" t="n">
+      <c r="A145" s="3" t="n">
         <v>147</v>
       </c>
-      <c r="B145" s="11" t="s">
-        <v>465</v>
-      </c>
-      <c r="C145" s="12"/>
+      <c r="B145" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="C145" s="3"/>
       <c r="D145" s="3" t="s">
         <v>387</v>
       </c>
@@ -7918,33 +7900,33 @@
       <c r="G145" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H145" s="11" t="s">
-        <v>466</v>
-      </c>
-      <c r="I145" s="12" t="n">
-        <v>172</v>
-      </c>
-      <c r="J145" s="12" t="s">
-        <v>437</v>
+      <c r="H145" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="I145" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="J145" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="K145" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="L145" s="14" t="n">
-        <v>-89.193359</v>
-      </c>
-      <c r="M145" s="12" t="n">
-        <v>13.685799</v>
+        <v>468</v>
+      </c>
+      <c r="L145" s="7" t="n">
+        <v>-89.183801</v>
+      </c>
+      <c r="M145" s="3" t="n">
+        <v>13.681814</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="12" t="n">
+      <c r="A146" s="3" t="n">
         <v>148</v>
       </c>
-      <c r="B146" s="11" t="s">
-        <v>468</v>
-      </c>
-      <c r="C146" s="12"/>
+      <c r="B146" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="C146" s="3"/>
       <c r="D146" s="3" t="s">
         <v>387</v>
       </c>
@@ -7957,33 +7939,33 @@
       <c r="G146" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H146" s="11" t="s">
-        <v>469</v>
-      </c>
-      <c r="I146" s="12" t="n">
-        <v>12</v>
-      </c>
-      <c r="J146" s="12" t="s">
+      <c r="H146" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="I146" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="J146" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K146" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="L146" s="14" t="n">
-        <v>-89.183801</v>
-      </c>
-      <c r="M146" s="12" t="n">
-        <v>13.681814</v>
+        <v>471</v>
+      </c>
+      <c r="L146" s="7" t="n">
+        <v>-89.201469</v>
+      </c>
+      <c r="M146" s="3" t="n">
+        <v>13.688991</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="12" t="n">
+      <c r="A147" s="3" t="n">
         <v>149</v>
       </c>
-      <c r="B147" s="11" t="s">
-        <v>471</v>
-      </c>
-      <c r="C147" s="12"/>
+      <c r="B147" s="10" t="s">
+        <v>472</v>
+      </c>
+      <c r="C147" s="3"/>
       <c r="D147" s="3" t="s">
         <v>387</v>
       </c>
@@ -7996,33 +7978,33 @@
       <c r="G147" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H147" s="11" t="s">
-        <v>472</v>
-      </c>
-      <c r="I147" s="12" t="n">
-        <v>19</v>
-      </c>
-      <c r="J147" s="12" t="s">
+      <c r="H147" s="10" t="s">
+        <v>473</v>
+      </c>
+      <c r="I147" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J147" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K147" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="L147" s="14" t="n">
-        <v>-89.201469</v>
-      </c>
-      <c r="M147" s="12" t="n">
-        <v>13.688991</v>
+        <v>20</v>
+      </c>
+      <c r="L147" s="7" t="n">
+        <v>-89.205442</v>
+      </c>
+      <c r="M147" s="3" t="n">
+        <v>13.714927</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="12" t="n">
+      <c r="A148" s="3" t="n">
         <v>150</v>
       </c>
-      <c r="B148" s="11" t="s">
+      <c r="B148" s="10" t="s">
         <v>474</v>
       </c>
-      <c r="C148" s="12"/>
+      <c r="C148" s="3"/>
       <c r="D148" s="3" t="s">
         <v>387</v>
       </c>
@@ -8035,33 +8017,33 @@
       <c r="G148" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H148" s="11" t="s">
+      <c r="H148" s="10" t="s">
         <v>475</v>
       </c>
-      <c r="I148" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="J148" s="12" t="s">
-        <v>391</v>
+      <c r="I148" s="3" t="n">
+        <v>66</v>
+      </c>
+      <c r="J148" s="3" t="s">
+        <v>476</v>
       </c>
       <c r="K148" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L148" s="14" t="n">
-        <v>-89.205442</v>
-      </c>
-      <c r="M148" s="12" t="n">
-        <v>13.714927</v>
+        <v>477</v>
+      </c>
+      <c r="L148" s="7" t="n">
+        <v>-89.188603</v>
+      </c>
+      <c r="M148" s="3" t="n">
+        <v>13.695563</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="12" t="n">
+      <c r="A149" s="3" t="n">
         <v>151</v>
       </c>
-      <c r="B149" s="11" t="s">
-        <v>476</v>
-      </c>
-      <c r="C149" s="12"/>
+      <c r="B149" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="C149" s="3"/>
       <c r="D149" s="3" t="s">
         <v>387</v>
       </c>
@@ -8074,33 +8056,33 @@
       <c r="G149" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H149" s="11" t="s">
-        <v>477</v>
-      </c>
-      <c r="I149" s="12" t="n">
-        <v>66</v>
-      </c>
-      <c r="J149" s="12" t="s">
-        <v>478</v>
+      <c r="H149" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="I149" s="3" t="n">
+        <v>63</v>
+      </c>
+      <c r="J149" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="K149" s="3" t="s">
-        <v>479</v>
-      </c>
-      <c r="L149" s="14" t="n">
-        <v>-89.188603</v>
-      </c>
-      <c r="M149" s="12" t="n">
-        <v>13.695563</v>
+        <v>20</v>
+      </c>
+      <c r="L149" s="7" t="n">
+        <v>-89.182415</v>
+      </c>
+      <c r="M149" s="3" t="n">
+        <v>13.702174</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="12" t="n">
+      <c r="A150" s="3" t="n">
         <v>152</v>
       </c>
-      <c r="B150" s="11" t="s">
+      <c r="B150" s="10" t="s">
         <v>480</v>
       </c>
-      <c r="C150" s="12"/>
+      <c r="C150" s="3"/>
       <c r="D150" s="3" t="s">
         <v>387</v>
       </c>
@@ -8113,33 +8095,33 @@
       <c r="G150" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H150" s="11" t="s">
+      <c r="H150" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="I150" s="12" t="n">
-        <v>63</v>
-      </c>
-      <c r="J150" s="12" t="s">
-        <v>391</v>
+      <c r="I150" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="J150" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="K150" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L150" s="14" t="n">
-        <v>-89.182415</v>
-      </c>
-      <c r="M150" s="12" t="n">
-        <v>13.702174</v>
+        <v>482</v>
+      </c>
+      <c r="L150" s="7" t="n">
+        <v>-89.185002</v>
+      </c>
+      <c r="M150" s="3" t="n">
+        <v>13.701283</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="12" t="n">
+      <c r="A151" s="3" t="n">
         <v>153</v>
       </c>
-      <c r="B151" s="11" t="s">
-        <v>482</v>
-      </c>
-      <c r="C151" s="12"/>
+      <c r="B151" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="C151" s="3"/>
       <c r="D151" s="3" t="s">
         <v>387</v>
       </c>
@@ -8152,33 +8134,33 @@
       <c r="G151" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H151" s="11" t="s">
-        <v>483</v>
-      </c>
-      <c r="I151" s="12" t="n">
-        <v>31</v>
-      </c>
-      <c r="J151" s="12" t="s">
-        <v>132</v>
+      <c r="H151" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="I151" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J151" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="K151" s="3" t="s">
-        <v>484</v>
-      </c>
-      <c r="L151" s="14" t="n">
-        <v>-89.185002</v>
-      </c>
-      <c r="M151" s="12" t="n">
-        <v>13.701283</v>
+        <v>485</v>
+      </c>
+      <c r="L151" s="7" t="n">
+        <v>-89.190761</v>
+      </c>
+      <c r="M151" s="3" t="n">
+        <v>13.716776</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="12" t="n">
+      <c r="A152" s="3" t="n">
         <v>154</v>
       </c>
-      <c r="B152" s="11" t="s">
-        <v>485</v>
-      </c>
-      <c r="C152" s="12"/>
+      <c r="B152" s="10" t="s">
+        <v>486</v>
+      </c>
+      <c r="C152" s="3"/>
       <c r="D152" s="3" t="s">
         <v>387</v>
       </c>
@@ -8191,33 +8173,33 @@
       <c r="G152" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H152" s="11" t="s">
-        <v>486</v>
-      </c>
-      <c r="I152" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J152" s="12" t="s">
-        <v>391</v>
+      <c r="H152" s="10" t="s">
+        <v>487</v>
+      </c>
+      <c r="I152" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="J152" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="K152" s="3" t="s">
-        <v>487</v>
-      </c>
-      <c r="L152" s="14" t="n">
-        <v>-89.190761</v>
-      </c>
-      <c r="M152" s="12" t="n">
-        <v>13.716776</v>
+        <v>488</v>
+      </c>
+      <c r="L152" s="7" t="n">
+        <v>-89.18091</v>
+      </c>
+      <c r="M152" s="3" t="n">
+        <v>13.713483</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="12" t="n">
+      <c r="A153" s="3" t="n">
         <v>155</v>
       </c>
-      <c r="B153" s="11" t="s">
-        <v>488</v>
-      </c>
-      <c r="C153" s="12"/>
+      <c r="B153" s="10" t="s">
+        <v>489</v>
+      </c>
+      <c r="C153" s="3"/>
       <c r="D153" s="3" t="s">
         <v>387</v>
       </c>
@@ -8230,33 +8212,33 @@
       <c r="G153" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H153" s="11" t="s">
-        <v>489</v>
-      </c>
-      <c r="I153" s="12" t="n">
-        <v>9</v>
-      </c>
-      <c r="J153" s="12" t="s">
-        <v>132</v>
+      <c r="H153" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="I153" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J153" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="K153" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="L153" s="14" t="n">
-        <v>-89.18091</v>
-      </c>
-      <c r="M153" s="12" t="n">
-        <v>13.713483</v>
+        <v>20</v>
+      </c>
+      <c r="L153" s="7" t="n">
+        <v>-89.184949</v>
+      </c>
+      <c r="M153" s="3" t="n">
+        <v>13.688765</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="12" t="n">
+      <c r="A154" s="3" t="n">
         <v>156</v>
       </c>
-      <c r="B154" s="11" t="s">
+      <c r="B154" s="10" t="s">
         <v>491</v>
       </c>
-      <c r="C154" s="12"/>
+      <c r="C154" s="3"/>
       <c r="D154" s="3" t="s">
         <v>387</v>
       </c>
@@ -8269,501 +8251,501 @@
       <c r="G154" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H154" s="11" t="s">
+      <c r="H154" s="10" t="s">
         <v>492</v>
       </c>
-      <c r="I154" s="12" t="n">
+      <c r="I154" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="L154" s="7" t="n">
+        <v>-89.20404</v>
+      </c>
+      <c r="M154" s="3" t="n">
+        <v>13.714081</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="3" t="n">
+        <v>157</v>
+      </c>
+      <c r="B155" s="10" t="s">
+        <v>494</v>
+      </c>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H155" s="10" t="s">
+        <v>495</v>
+      </c>
+      <c r="I155" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J155" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K155" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="L155" s="7" t="n">
+        <v>-89.243008</v>
+      </c>
+      <c r="M155" s="3" t="n">
+        <v>13.690646</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="3" t="n">
+        <v>158</v>
+      </c>
+      <c r="B156" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="C156" s="3"/>
+      <c r="D156" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H156" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="I156" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J156" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K156" s="3" t="s">
+        <v>499</v>
+      </c>
+      <c r="L156" s="7" t="n">
+        <v>-89.245457</v>
+      </c>
+      <c r="M156" s="3" t="n">
+        <v>13.70524</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="3" t="n">
+        <v>159</v>
+      </c>
+      <c r="B157" s="10" t="s">
+        <v>500</v>
+      </c>
+      <c r="C157" s="3"/>
+      <c r="D157" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H157" s="10" t="s">
+        <v>501</v>
+      </c>
+      <c r="I157" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="J157" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K157" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="L157" s="7" t="n">
+        <v>-89.222581</v>
+      </c>
+      <c r="M157" s="3" t="n">
+        <v>13.704889</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="3" t="n">
+        <v>160</v>
+      </c>
+      <c r="B158" s="10" t="s">
+        <v>503</v>
+      </c>
+      <c r="C158" s="3"/>
+      <c r="D158" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H158" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="I158" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J158" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K158" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="L158" s="7" t="n">
+        <v>-89.238696</v>
+      </c>
+      <c r="M158" s="3" t="n">
+        <v>13.709291</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="3" t="n">
+        <v>161</v>
+      </c>
+      <c r="B159" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="C159" s="3"/>
+      <c r="D159" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G159" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H159" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="I159" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="J154" s="12" t="s">
+      <c r="J159" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="K154" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L154" s="14" t="n">
-        <v>-89.184949</v>
-      </c>
-      <c r="M154" s="12" t="n">
-        <v>13.688765</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="12" t="n">
-        <v>157</v>
-      </c>
-      <c r="B155" s="11" t="s">
-        <v>493</v>
-      </c>
-      <c r="C155" s="12"/>
-      <c r="D155" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="E155" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F155" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G155" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H155" s="11" t="s">
-        <v>494</v>
-      </c>
-      <c r="I155" s="12" t="n">
-        <v>5</v>
-      </c>
-      <c r="J155" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="K155" s="3" t="s">
-        <v>495</v>
-      </c>
-      <c r="L155" s="14" t="n">
-        <v>-89.20404</v>
-      </c>
-      <c r="M155" s="12" t="n">
-        <v>13.714081</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="12" t="n">
-        <v>158</v>
-      </c>
-      <c r="B156" s="11" t="s">
-        <v>496</v>
-      </c>
-      <c r="C156" s="12"/>
-      <c r="D156" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E156" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F156" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G156" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H156" s="11" t="s">
-        <v>497</v>
-      </c>
-      <c r="I156" s="12" t="n">
+      <c r="K159" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="L159" s="7" t="n">
+        <v>-89.227664</v>
+      </c>
+      <c r="M159" s="3" t="n">
+        <v>13.70214</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="3" t="n">
+        <v>162</v>
+      </c>
+      <c r="B160" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="C160" s="3"/>
+      <c r="D160" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H160" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="I160" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="J156" s="12" t="s">
+      <c r="J160" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="K156" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="L156" s="14" t="n">
-        <v>-89.243008</v>
-      </c>
-      <c r="M156" s="12" t="n">
-        <v>13.690646</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="12" t="n">
-        <v>159</v>
-      </c>
-      <c r="B157" s="11" t="s">
-        <v>499</v>
-      </c>
-      <c r="C157" s="12"/>
-      <c r="D157" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F157" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G157" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H157" s="11" t="s">
-        <v>500</v>
-      </c>
-      <c r="I157" s="12" t="n">
+      <c r="K160" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="L160" s="7" t="n">
+        <v>-89.253597</v>
+      </c>
+      <c r="M160" s="3" t="n">
+        <v>13.707933</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="3" t="n">
+        <v>163</v>
+      </c>
+      <c r="B161" s="10" t="s">
+        <v>512</v>
+      </c>
+      <c r="C161" s="3"/>
+      <c r="D161" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G161" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H161" s="10" t="s">
+        <v>513</v>
+      </c>
+      <c r="I161" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="J161" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K161" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="L161" s="7" t="n">
+        <v>-89.221442</v>
+      </c>
+      <c r="M161" s="3" t="n">
+        <v>13.702451</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="3" t="n">
+        <v>164</v>
+      </c>
+      <c r="B162" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="C162" s="3"/>
+      <c r="D162" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G162" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H162" s="10" t="s">
+        <v>516</v>
+      </c>
+      <c r="I162" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="J162" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K162" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="L162" s="7" t="n">
+        <v>-89.218784</v>
+      </c>
+      <c r="M162" s="3" t="n">
+        <v>13.705245</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="3" t="n">
+        <v>165</v>
+      </c>
+      <c r="B163" s="10" t="s">
+        <v>518</v>
+      </c>
+      <c r="C163" s="3"/>
+      <c r="D163" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G163" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H163" s="10" t="s">
+        <v>519</v>
+      </c>
+      <c r="I163" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="J163" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K163" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="L163" s="7" t="n">
+        <v>-89.178321</v>
+      </c>
+      <c r="M163" s="3" t="n">
+        <v>13.700803</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="3" t="n">
+        <v>166</v>
+      </c>
+      <c r="B164" s="10" t="s">
+        <v>521</v>
+      </c>
+      <c r="C164" s="3"/>
+      <c r="D164" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H164" s="10" t="s">
+        <v>522</v>
+      </c>
+      <c r="I164" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J164" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K164" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="L164" s="7" t="n">
+        <v>-89.235271</v>
+      </c>
+      <c r="M164" s="3" t="n">
+        <v>13.705298</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="3" t="n">
+        <v>167</v>
+      </c>
+      <c r="B165" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="C165" s="3"/>
+      <c r="D165" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H165" s="10" t="s">
+        <v>525</v>
+      </c>
+      <c r="I165" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="J157" s="12" t="s">
+      <c r="J165" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="K157" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="L157" s="14" t="n">
-        <v>-89.245457</v>
-      </c>
-      <c r="M157" s="12" t="n">
-        <v>13.70524</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="12" t="n">
-        <v>160</v>
-      </c>
-      <c r="B158" s="11" t="s">
-        <v>502</v>
-      </c>
-      <c r="C158" s="12"/>
-      <c r="D158" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E158" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F158" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G158" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H158" s="11" t="s">
-        <v>503</v>
-      </c>
-      <c r="I158" s="12" t="n">
-        <v>13</v>
-      </c>
-      <c r="J158" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="K158" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="L158" s="14" t="n">
-        <v>-89.222581</v>
-      </c>
-      <c r="M158" s="12" t="n">
-        <v>13.704889</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="12" t="n">
-        <v>161</v>
-      </c>
-      <c r="B159" s="11" t="s">
-        <v>505</v>
-      </c>
-      <c r="C159" s="12"/>
-      <c r="D159" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E159" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F159" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G159" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H159" s="11" t="s">
-        <v>506</v>
-      </c>
-      <c r="I159" s="12" t="n">
-        <v>7</v>
-      </c>
-      <c r="J159" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="K159" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="L159" s="14" t="n">
-        <v>-89.238696</v>
-      </c>
-      <c r="M159" s="12" t="n">
-        <v>13.709291</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="12" t="n">
-        <v>162</v>
-      </c>
-      <c r="B160" s="11" t="s">
-        <v>508</v>
-      </c>
-      <c r="C160" s="12"/>
-      <c r="D160" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E160" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F160" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G160" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H160" s="11" t="s">
-        <v>509</v>
-      </c>
-      <c r="I160" s="12" t="n">
-        <v>4</v>
-      </c>
-      <c r="J160" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="K160" s="3" t="s">
-        <v>510</v>
-      </c>
-      <c r="L160" s="14" t="n">
-        <v>-89.227664</v>
-      </c>
-      <c r="M160" s="12" t="n">
-        <v>13.70214</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="12" t="n">
-        <v>163</v>
-      </c>
-      <c r="B161" s="11" t="s">
-        <v>511</v>
-      </c>
-      <c r="C161" s="12"/>
-      <c r="D161" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E161" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F161" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G161" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H161" s="11" t="s">
-        <v>512</v>
-      </c>
-      <c r="I161" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J161" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="K161" s="3" t="s">
-        <v>513</v>
-      </c>
-      <c r="L161" s="14" t="n">
-        <v>-89.253597</v>
-      </c>
-      <c r="M161" s="12" t="n">
-        <v>13.707933</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="12" t="n">
-        <v>164</v>
-      </c>
-      <c r="B162" s="11" t="s">
-        <v>514</v>
-      </c>
-      <c r="C162" s="12"/>
-      <c r="D162" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F162" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G162" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H162" s="11" t="s">
-        <v>515</v>
-      </c>
-      <c r="I162" s="12" t="n">
-        <v>10</v>
-      </c>
-      <c r="J162" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="K162" s="3" t="s">
-        <v>516</v>
-      </c>
-      <c r="L162" s="14" t="n">
-        <v>-89.221442</v>
-      </c>
-      <c r="M162" s="12" t="n">
-        <v>13.702451</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="12" t="n">
-        <v>165</v>
-      </c>
-      <c r="B163" s="11" t="s">
-        <v>517</v>
-      </c>
-      <c r="C163" s="12"/>
-      <c r="D163" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F163" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G163" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H163" s="11" t="s">
-        <v>518</v>
-      </c>
-      <c r="I163" s="12" t="n">
-        <v>23</v>
-      </c>
-      <c r="J163" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="K163" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="L163" s="14" t="n">
-        <v>-89.218784</v>
-      </c>
-      <c r="M163" s="12" t="n">
-        <v>13.705245</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="12" t="n">
-        <v>166</v>
-      </c>
-      <c r="B164" s="11" t="s">
-        <v>520</v>
-      </c>
-      <c r="C164" s="12"/>
-      <c r="D164" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E164" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F164" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G164" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H164" s="11" t="s">
-        <v>521</v>
-      </c>
-      <c r="I164" s="12" t="n">
-        <v>8</v>
-      </c>
-      <c r="J164" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="K164" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="L164" s="14" t="n">
-        <v>-89.178321</v>
-      </c>
-      <c r="M164" s="12" t="n">
-        <v>13.700803</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="12" t="n">
-        <v>167</v>
-      </c>
-      <c r="B165" s="11" t="s">
-        <v>523</v>
-      </c>
-      <c r="C165" s="12"/>
-      <c r="D165" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F165" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G165" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H165" s="11" t="s">
-        <v>524</v>
-      </c>
-      <c r="I165" s="12" t="n">
+      <c r="K165" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="L165" s="7" t="n">
+        <v>-89.210737</v>
+      </c>
+      <c r="M165" s="3" t="n">
+        <v>13.707132</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="3" t="n">
+        <v>168</v>
+      </c>
+      <c r="B166" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C166" s="3"/>
+      <c r="D166" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H166" s="10" t="s">
+        <v>527</v>
+      </c>
+      <c r="I166" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="J165" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="K165" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="L165" s="14" t="n">
-        <v>-89.235271</v>
-      </c>
-      <c r="M165" s="12" t="n">
-        <v>13.705298</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="12" t="n">
-        <v>168</v>
-      </c>
-      <c r="B166" s="11" t="s">
-        <v>526</v>
-      </c>
-      <c r="C166" s="12"/>
-      <c r="D166" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E166" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F166" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G166" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H166" s="11" t="s">
-        <v>527</v>
-      </c>
-      <c r="I166" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J166" s="12" t="s">
+      <c r="J166" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K166" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="L166" s="14" t="n">
-        <v>-89.210737</v>
-      </c>
-      <c r="M166" s="12" t="n">
-        <v>13.707132</v>
+      <c r="L166" s="7" t="n">
+        <v>-89.232965</v>
+      </c>
+      <c r="M166" s="3" t="n">
+        <v>13.693469</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="12" t="n">
+      <c r="A167" s="3" t="n">
         <v>169</v>
       </c>
-      <c r="B167" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C167" s="12"/>
+      <c r="B167" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C167" s="3"/>
       <c r="D167" s="3" t="s">
         <v>15</v>
       </c>
@@ -8776,111 +8758,111 @@
       <c r="G167" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H167" s="11" t="s">
+      <c r="H167" s="10" t="s">
         <v>529</v>
       </c>
-      <c r="I167" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="J167" s="12" t="s">
+      <c r="I167" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J167" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K167" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L167" s="7" t="n">
+        <v>-89.23929</v>
+      </c>
+      <c r="M167" s="3" t="n">
+        <v>13.695543</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="3" t="n">
+        <v>170</v>
+      </c>
+      <c r="B168" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C168" s="3"/>
+      <c r="D168" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H168" s="10" t="s">
         <v>530</v>
       </c>
-      <c r="L167" s="14" t="n">
-        <v>-89.232965</v>
-      </c>
-      <c r="M167" s="12" t="n">
-        <v>13.693469</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="12" t="n">
-        <v>170</v>
-      </c>
-      <c r="B168" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="C168" s="12"/>
-      <c r="D168" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E168" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F168" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G168" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H168" s="11" t="s">
+      <c r="I168" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J168" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K168" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="I168" s="12" t="n">
+      <c r="L168" s="7" t="n">
+        <v>-89.230805</v>
+      </c>
+      <c r="M168" s="3" t="n">
+        <v>13.696263</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="3" t="n">
+        <v>171</v>
+      </c>
+      <c r="B169" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C169" s="3"/>
+      <c r="D169" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H169" s="10" t="s">
+        <v>532</v>
+      </c>
+      <c r="I169" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="J168" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="K168" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L168" s="14" t="n">
-        <v>-89.23929</v>
-      </c>
-      <c r="M168" s="12" t="n">
-        <v>13.695543</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="12" t="n">
-        <v>171</v>
-      </c>
-      <c r="B169" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="C169" s="12"/>
-      <c r="D169" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F169" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G169" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H169" s="11" t="s">
-        <v>532</v>
-      </c>
-      <c r="I169" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J169" s="12" t="s">
+      <c r="J169" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K169" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="L169" s="14" t="n">
-        <v>-89.230805</v>
-      </c>
-      <c r="M169" s="12" t="n">
-        <v>13.696263</v>
+      <c r="L169" s="7" t="n">
+        <v>-89.256372</v>
+      </c>
+      <c r="M169" s="3" t="n">
+        <v>13.7117</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="12" t="n">
+      <c r="A170" s="3" t="n">
         <v>172</v>
       </c>
-      <c r="B170" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="C170" s="12"/>
+      <c r="B170" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C170" s="3"/>
       <c r="D170" s="3" t="s">
         <v>15</v>
       </c>
@@ -8893,33 +8875,33 @@
       <c r="G170" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H170" s="11" t="s">
+      <c r="H170" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="I170" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J170" s="12" t="s">
+      <c r="I170" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J170" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K170" s="3" t="s">
         <v>535</v>
       </c>
-      <c r="L170" s="14" t="n">
-        <v>-89.256372</v>
-      </c>
-      <c r="M170" s="12" t="n">
-        <v>13.7117</v>
+      <c r="L170" s="7" t="n">
+        <v>-89.223832</v>
+      </c>
+      <c r="M170" s="3" t="n">
+        <v>13.697799</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="12" t="n">
+      <c r="A171" s="3" t="n">
         <v>173</v>
       </c>
-      <c r="B171" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="C171" s="12"/>
+      <c r="B171" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C171" s="3"/>
       <c r="D171" s="3" t="s">
         <v>15</v>
       </c>
@@ -8932,33 +8914,33 @@
       <c r="G171" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H171" s="11" t="s">
+      <c r="H171" s="10" t="s">
         <v>536</v>
       </c>
-      <c r="I171" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="J171" s="12" t="s">
+      <c r="I171" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="J171" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K171" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="L171" s="14" t="n">
-        <v>-89.223832</v>
-      </c>
-      <c r="M171" s="12" t="n">
-        <v>13.697799</v>
+      <c r="L171" s="7" t="n">
+        <v>-89.210209</v>
+      </c>
+      <c r="M171" s="3" t="n">
+        <v>13.702619</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="12" t="n">
+      <c r="A172" s="3" t="n">
         <v>174</v>
       </c>
-      <c r="B172" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="C172" s="12"/>
+      <c r="B172" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C172" s="3"/>
       <c r="D172" s="3" t="s">
         <v>15</v>
       </c>
@@ -8971,33 +8953,33 @@
       <c r="G172" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H172" s="11" t="s">
+      <c r="H172" s="10" t="s">
         <v>538</v>
       </c>
-      <c r="I172" s="12" t="n">
-        <v>20</v>
-      </c>
-      <c r="J172" s="12" t="s">
+      <c r="I172" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J172" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K172" s="3" t="s">
         <v>539</v>
       </c>
-      <c r="L172" s="14" t="n">
-        <v>-89.210209</v>
-      </c>
-      <c r="M172" s="12" t="n">
-        <v>13.702619</v>
+      <c r="L172" s="7" t="n">
+        <v>-89.240028</v>
+      </c>
+      <c r="M172" s="3" t="n">
+        <v>13.703282</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="12" t="n">
+      <c r="A173" s="3" t="n">
         <v>175</v>
       </c>
-      <c r="B173" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="C173" s="12"/>
+      <c r="B173" s="10" t="s">
+        <v>540</v>
+      </c>
+      <c r="C173" s="3"/>
       <c r="D173" s="3" t="s">
         <v>15</v>
       </c>
@@ -9010,33 +8992,33 @@
       <c r="G173" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H173" s="11" t="s">
-        <v>540</v>
-      </c>
-      <c r="I173" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J173" s="12" t="s">
-        <v>391</v>
+      <c r="H173" s="10" t="s">
+        <v>541</v>
+      </c>
+      <c r="I173" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="J173" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="K173" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="L173" s="14" t="n">
-        <v>-89.240028</v>
-      </c>
-      <c r="M173" s="12" t="n">
-        <v>13.703282</v>
+        <v>542</v>
+      </c>
+      <c r="L173" s="7" t="n">
+        <v>-89.24276</v>
+      </c>
+      <c r="M173" s="3" t="n">
+        <v>13.68203</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="12" t="n">
+      <c r="A174" s="3" t="n">
         <v>176</v>
       </c>
-      <c r="B174" s="11" t="s">
-        <v>542</v>
-      </c>
-      <c r="C174" s="12"/>
+      <c r="B174" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C174" s="3"/>
       <c r="D174" s="3" t="s">
         <v>15</v>
       </c>
@@ -9049,33 +9031,33 @@
       <c r="G174" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H174" s="11" t="s">
+      <c r="H174" s="10" t="s">
         <v>543</v>
       </c>
-      <c r="I174" s="12" t="n">
-        <v>12</v>
-      </c>
-      <c r="J174" s="12" t="s">
+      <c r="I174" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="J174" s="3" t="s">
         <v>132</v>
       </c>
       <c r="K174" s="3" t="s">
         <v>544</v>
       </c>
-      <c r="L174" s="14" t="n">
-        <v>-89.24224</v>
-      </c>
-      <c r="M174" s="12" t="n">
-        <v>13.680559</v>
+      <c r="L174" s="7" t="n">
+        <v>-89.203052</v>
+      </c>
+      <c r="M174" s="3" t="n">
+        <v>13.714146</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="12" t="n">
+      <c r="A175" s="3" t="n">
         <v>177</v>
       </c>
-      <c r="B175" s="11" t="s">
-        <v>215</v>
-      </c>
-      <c r="C175" s="12"/>
+      <c r="B175" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C175" s="3"/>
       <c r="D175" s="3" t="s">
         <v>15</v>
       </c>
@@ -9088,33 +9070,33 @@
       <c r="G175" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H175" s="11" t="s">
+      <c r="H175" s="10" t="s">
         <v>545</v>
       </c>
-      <c r="I175" s="12" t="n">
-        <v>6</v>
-      </c>
-      <c r="J175" s="12" t="s">
-        <v>132</v>
+      <c r="I175" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J175" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="K175" s="3" t="s">
         <v>546</v>
       </c>
-      <c r="L175" s="14" t="n">
-        <v>-89.203052</v>
-      </c>
-      <c r="M175" s="12" t="n">
-        <v>13.714146</v>
+      <c r="L175" s="7" t="n">
+        <v>-89.191294</v>
+      </c>
+      <c r="M175" s="3" t="n">
+        <v>13.706586</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="12" t="n">
+      <c r="A176" s="3" t="n">
         <v>178</v>
       </c>
-      <c r="B176" s="11" t="s">
-        <v>218</v>
-      </c>
-      <c r="C176" s="12"/>
+      <c r="B176" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C176" s="3"/>
       <c r="D176" s="3" t="s">
         <v>15</v>
       </c>
@@ -9127,33 +9109,33 @@
       <c r="G176" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H176" s="11" t="s">
+      <c r="H176" s="10" t="s">
         <v>547</v>
       </c>
-      <c r="I176" s="12" t="n">
-        <v>3</v>
-      </c>
-      <c r="J176" s="12" t="s">
+      <c r="I176" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="J176" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K176" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="L176" s="14" t="n">
-        <v>-89.191294</v>
-      </c>
-      <c r="M176" s="12" t="n">
-        <v>13.706586</v>
+      <c r="L176" s="7" t="n">
+        <v>-89.191279</v>
+      </c>
+      <c r="M176" s="3" t="n">
+        <v>13.680828</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="12" t="n">
+      <c r="A177" s="3" t="n">
         <v>179</v>
       </c>
-      <c r="B177" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="C177" s="12"/>
+      <c r="B177" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C177" s="3"/>
       <c r="D177" s="3" t="s">
         <v>15</v>
       </c>
@@ -9166,33 +9148,33 @@
       <c r="G177" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H177" s="11" t="s">
+      <c r="H177" s="10" t="s">
         <v>549</v>
       </c>
-      <c r="I177" s="12" t="n">
-        <v>11</v>
-      </c>
-      <c r="J177" s="12" t="s">
+      <c r="I177" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J177" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K177" s="3" t="s">
         <v>550</v>
       </c>
-      <c r="L177" s="14" t="n">
-        <v>-89.191279</v>
-      </c>
-      <c r="M177" s="12" t="n">
-        <v>13.680828</v>
+      <c r="L177" s="7" t="n">
+        <v>-89.19128</v>
+      </c>
+      <c r="M177" s="3" t="n">
+        <v>13.683268</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="12" t="n">
+      <c r="A178" s="3" t="n">
         <v>180</v>
       </c>
-      <c r="B178" s="11" t="s">
-        <v>224</v>
-      </c>
-      <c r="C178" s="12"/>
+      <c r="B178" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="C178" s="3"/>
       <c r="D178" s="3" t="s">
         <v>15</v>
       </c>
@@ -9205,33 +9187,33 @@
       <c r="G178" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H178" s="11" t="s">
+      <c r="H178" s="10" t="s">
         <v>551</v>
       </c>
-      <c r="I178" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J178" s="12" t="s">
+      <c r="I178" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="J178" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K178" s="3" t="s">
         <v>552</v>
       </c>
-      <c r="L178" s="14" t="n">
-        <v>-89.19128</v>
-      </c>
-      <c r="M178" s="12" t="n">
-        <v>13.683268</v>
+      <c r="L178" s="7" t="n">
+        <v>-89.229835</v>
+      </c>
+      <c r="M178" s="3" t="n">
+        <v>13.697852</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="12" t="n">
+      <c r="A179" s="3" t="n">
         <v>181</v>
       </c>
-      <c r="B179" s="11" t="s">
-        <v>226</v>
-      </c>
-      <c r="C179" s="12"/>
+      <c r="B179" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="C179" s="3"/>
       <c r="D179" s="3" t="s">
         <v>15</v>
       </c>
@@ -9244,38 +9226,38 @@
       <c r="G179" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H179" s="11" t="s">
+      <c r="H179" s="10" t="s">
         <v>553</v>
       </c>
-      <c r="I179" s="12" t="n">
-        <v>17</v>
-      </c>
-      <c r="J179" s="12" t="s">
-        <v>391</v>
+      <c r="I179" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="J179" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="K179" s="3" t="s">
         <v>554</v>
       </c>
-      <c r="L179" s="14" t="n">
-        <v>-89.229835</v>
-      </c>
-      <c r="M179" s="12" t="n">
-        <v>13.697852</v>
+      <c r="L179" s="7" t="n">
+        <v>-89.228287</v>
+      </c>
+      <c r="M179" s="3" t="n">
+        <v>13.674987</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="12" t="n">
+      <c r="A180" s="3" t="n">
         <v>182</v>
       </c>
-      <c r="B180" s="11" t="s">
-        <v>228</v>
-      </c>
-      <c r="C180" s="12"/>
+      <c r="B180" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="C180" s="3"/>
       <c r="D180" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E180" s="3" t="s">
-        <v>16</v>
+        <v>108</v>
       </c>
       <c r="F180" s="3" t="s">
         <v>17</v>
@@ -9283,38 +9265,38 @@
       <c r="G180" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H180" s="11" t="s">
+      <c r="H180" s="10" t="s">
         <v>555</v>
       </c>
-      <c r="I180" s="12" t="n">
-        <v>13</v>
-      </c>
-      <c r="J180" s="12" t="s">
-        <v>132</v>
+      <c r="I180" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J180" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="K180" s="3" t="s">
         <v>556</v>
       </c>
-      <c r="L180" s="14" t="n">
-        <v>-89.228287</v>
-      </c>
-      <c r="M180" s="12" t="n">
-        <v>13.674987</v>
+      <c r="L180" s="7" t="n">
+        <v>-89.188573</v>
+      </c>
+      <c r="M180" s="3" t="n">
+        <v>13.689968</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="12" t="n">
+      <c r="A181" s="3" t="n">
         <v>183</v>
       </c>
-      <c r="B181" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="C181" s="12"/>
+      <c r="B181" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C181" s="3"/>
       <c r="D181" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E181" s="3" t="s">
-        <v>108</v>
+        <v>16</v>
       </c>
       <c r="F181" s="3" t="s">
         <v>17</v>
@@ -9322,35 +9304,35 @@
       <c r="G181" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H181" s="11" t="s">
+      <c r="H181" s="10" t="s">
         <v>557</v>
       </c>
-      <c r="I181" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="J181" s="12" t="s">
+      <c r="I181" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J181" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K181" s="3" t="s">
         <v>558</v>
       </c>
-      <c r="L181" s="14" t="n">
-        <v>-89.188573</v>
-      </c>
-      <c r="M181" s="12" t="n">
-        <v>13.689968</v>
+      <c r="L181" s="7" t="n">
+        <v>-89.187146</v>
+      </c>
+      <c r="M181" s="3" t="n">
+        <v>13.702182</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="12" t="n">
+      <c r="A182" s="3" t="n">
         <v>184</v>
       </c>
-      <c r="B182" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C182" s="12"/>
+      <c r="B182" s="10" t="s">
+        <v>559</v>
+      </c>
+      <c r="C182" s="3"/>
       <c r="D182" s="3" t="s">
-        <v>15</v>
+        <v>387</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>16</v>
@@ -9361,35 +9343,35 @@
       <c r="G182" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H182" s="11" t="s">
-        <v>559</v>
-      </c>
-      <c r="I182" s="12" t="n">
-        <v>4</v>
-      </c>
-      <c r="J182" s="12" t="s">
+      <c r="H182" s="10" t="s">
+        <v>560</v>
+      </c>
+      <c r="I182" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J182" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K182" s="3" t="s">
-        <v>560</v>
-      </c>
-      <c r="L182" s="14" t="n">
-        <v>-89.187146</v>
-      </c>
-      <c r="M182" s="12" t="n">
-        <v>13.702182</v>
+        <v>561</v>
+      </c>
+      <c r="L182" s="7" t="n">
+        <v>-89.190549</v>
+      </c>
+      <c r="M182" s="3" t="n">
+        <v>13.702856</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="12" t="n">
+      <c r="A183" s="3" t="n">
         <v>185</v>
       </c>
-      <c r="B183" s="11" t="s">
-        <v>561</v>
-      </c>
-      <c r="C183" s="12"/>
+      <c r="B183" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C183" s="3"/>
       <c r="D183" s="3" t="s">
-        <v>387</v>
+        <v>15</v>
       </c>
       <c r="E183" s="3" t="s">
         <v>16</v>
@@ -9400,33 +9382,33 @@
       <c r="G183" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H183" s="11" t="s">
+      <c r="H183" s="10" t="s">
         <v>562</v>
       </c>
-      <c r="I183" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="J183" s="12" t="s">
+      <c r="I183" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J183" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K183" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="L183" s="14" t="n">
-        <v>-89.190549</v>
-      </c>
-      <c r="M183" s="12" t="n">
-        <v>13.702856</v>
+      <c r="L183" s="7" t="n">
+        <v>-89.217358</v>
+      </c>
+      <c r="M183" s="3" t="n">
+        <v>13.722426</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="12" t="n">
+      <c r="A184" s="3" t="n">
         <v>186</v>
       </c>
-      <c r="B184" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="C184" s="12"/>
+      <c r="B184" s="10" t="s">
+        <v>240</v>
+      </c>
+      <c r="C184" s="3"/>
       <c r="D184" s="3" t="s">
         <v>15</v>
       </c>
@@ -9439,33 +9421,33 @@
       <c r="G184" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H184" s="11" t="s">
+      <c r="H184" s="10" t="s">
         <v>564</v>
       </c>
-      <c r="I184" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="J184" s="12" t="s">
+      <c r="I184" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="J184" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K184" s="3" t="s">
         <v>565</v>
       </c>
-      <c r="L184" s="14" t="n">
-        <v>-89.217358</v>
-      </c>
-      <c r="M184" s="12" t="n">
-        <v>13.722426</v>
+      <c r="L184" s="7" t="n">
+        <v>-89.209983</v>
+      </c>
+      <c r="M184" s="3" t="n">
+        <v>13.7149</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="12" t="n">
+      <c r="A185" s="3" t="n">
         <v>187</v>
       </c>
-      <c r="B185" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="C185" s="12"/>
+      <c r="B185" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C185" s="3"/>
       <c r="D185" s="3" t="s">
         <v>15</v>
       </c>
@@ -9478,33 +9460,33 @@
       <c r="G185" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H185" s="11" t="s">
+      <c r="H185" s="10" t="s">
         <v>566</v>
       </c>
-      <c r="I185" s="12" t="n">
-        <v>3</v>
-      </c>
-      <c r="J185" s="12" t="s">
+      <c r="I185" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J185" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K185" s="3" t="s">
         <v>567</v>
       </c>
-      <c r="L185" s="14" t="n">
-        <v>-89.209983</v>
-      </c>
-      <c r="M185" s="12" t="n">
-        <v>13.7149</v>
+      <c r="L185" s="7" t="n">
+        <v>-89.204366</v>
+      </c>
+      <c r="M185" s="3" t="n">
+        <v>13.708281</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="12" t="n">
+      <c r="A186" s="3" t="n">
         <v>188</v>
       </c>
-      <c r="B186" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="C186" s="12"/>
+      <c r="B186" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="C186" s="3"/>
       <c r="D186" s="3" t="s">
         <v>15</v>
       </c>
@@ -9517,33 +9499,33 @@
       <c r="G186" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H186" s="11" t="s">
+      <c r="H186" s="10" t="s">
         <v>568</v>
       </c>
-      <c r="I186" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="J186" s="12" t="s">
+      <c r="I186" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="J186" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K186" s="3" t="s">
         <v>569</v>
       </c>
-      <c r="L186" s="14" t="n">
-        <v>-89.204366</v>
-      </c>
-      <c r="M186" s="12" t="n">
-        <v>13.708281</v>
+      <c r="L186" s="7" t="n">
+        <v>-89.206</v>
+      </c>
+      <c r="M186" s="3" t="n">
+        <v>13.706295</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="12" t="n">
+      <c r="A187" s="3" t="n">
         <v>189</v>
       </c>
-      <c r="B187" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="C187" s="12"/>
+      <c r="B187" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C187" s="3"/>
       <c r="D187" s="3" t="s">
         <v>15</v>
       </c>
@@ -9556,33 +9538,33 @@
       <c r="G187" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H187" s="11" t="s">
+      <c r="H187" s="10" t="s">
         <v>570</v>
       </c>
-      <c r="I187" s="12" t="n">
-        <v>5</v>
-      </c>
-      <c r="J187" s="12" t="s">
+      <c r="I187" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J187" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K187" s="3" t="s">
         <v>571</v>
       </c>
-      <c r="L187" s="14" t="n">
-        <v>-89.206</v>
-      </c>
-      <c r="M187" s="12" t="n">
-        <v>13.706295</v>
+      <c r="L187" s="7" t="n">
+        <v>-89.204842</v>
+      </c>
+      <c r="M187" s="3" t="n">
+        <v>13.709922</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="12" t="n">
+      <c r="A188" s="3" t="n">
         <v>190</v>
       </c>
-      <c r="B188" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="C188" s="12"/>
+      <c r="B188" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C188" s="3"/>
       <c r="D188" s="3" t="s">
         <v>15</v>
       </c>
@@ -9595,33 +9577,33 @@
       <c r="G188" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H188" s="11" t="s">
+      <c r="H188" s="10" t="s">
         <v>572</v>
       </c>
-      <c r="I188" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J188" s="12" t="s">
+      <c r="I188" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J188" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K188" s="3" t="s">
         <v>573</v>
       </c>
-      <c r="L188" s="14" t="n">
-        <v>-89.204842</v>
-      </c>
-      <c r="M188" s="12" t="n">
-        <v>13.709922</v>
+      <c r="L188" s="7" t="n">
+        <v>-89.227099</v>
+      </c>
+      <c r="M188" s="3" t="n">
+        <v>13.722103</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="12" t="n">
+      <c r="A189" s="3" t="n">
         <v>191</v>
       </c>
-      <c r="B189" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="C189" s="12"/>
+      <c r="B189" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="C189" s="3"/>
       <c r="D189" s="3" t="s">
         <v>15</v>
       </c>
@@ -9634,33 +9616,33 @@
       <c r="G189" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H189" s="11" t="s">
+      <c r="H189" s="10" t="s">
         <v>574</v>
       </c>
-      <c r="I189" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="J189" s="12" t="s">
-        <v>391</v>
+      <c r="I189" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J189" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="K189" s="3" t="s">
         <v>575</v>
       </c>
-      <c r="L189" s="14" t="n">
-        <v>-89.227099</v>
-      </c>
-      <c r="M189" s="12" t="n">
-        <v>13.722103</v>
+      <c r="L189" s="7" t="n">
+        <v>-89.212439</v>
+      </c>
+      <c r="M189" s="3" t="n">
+        <v>13.724179</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="12" t="n">
+      <c r="A190" s="3" t="n">
         <v>192</v>
       </c>
-      <c r="B190" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="C190" s="12"/>
+      <c r="B190" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C190" s="3"/>
       <c r="D190" s="3" t="s">
         <v>15</v>
       </c>
@@ -9673,33 +9655,33 @@
       <c r="G190" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H190" s="11" t="s">
+      <c r="H190" s="10" t="s">
         <v>576</v>
       </c>
-      <c r="I190" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J190" s="12" t="s">
-        <v>132</v>
+      <c r="I190" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="J190" s="3" t="s">
+        <v>391</v>
       </c>
       <c r="K190" s="3" t="s">
         <v>577</v>
       </c>
-      <c r="L190" s="14" t="n">
-        <v>-89.212439</v>
-      </c>
-      <c r="M190" s="12" t="n">
-        <v>13.724179</v>
+      <c r="L190" s="7" t="n">
+        <v>-89.225903</v>
+      </c>
+      <c r="M190" s="3" t="n">
+        <v>13.718272</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="12" t="n">
+      <c r="A191" s="3" t="n">
         <v>193</v>
       </c>
-      <c r="B191" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="C191" s="12"/>
+      <c r="B191" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C191" s="3"/>
       <c r="D191" s="3" t="s">
         <v>15</v>
       </c>
@@ -9712,61 +9694,22 @@
       <c r="G191" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H191" s="11" t="s">
-        <v>578</v>
-      </c>
-      <c r="I191" s="12" t="n">
-        <v>4</v>
-      </c>
-      <c r="J191" s="12" t="s">
+      <c r="H191" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="I191" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="J191" s="3" t="s">
         <v>391</v>
       </c>
       <c r="K191" s="3" t="s">
-        <v>579</v>
-      </c>
-      <c r="L191" s="14" t="n">
-        <v>-89.225903</v>
-      </c>
-      <c r="M191" s="12" t="n">
-        <v>13.718272</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="12" t="n">
-        <v>194</v>
-      </c>
-      <c r="B192" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="C192" s="12"/>
-      <c r="D192" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E192" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F192" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G192" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H192" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="I192" s="12" t="n">
-        <v>9</v>
-      </c>
-      <c r="J192" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="K192" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="L192" s="14" t="n">
+      <c r="L191" s="7" t="n">
         <v>-89.216085</v>
       </c>
-      <c r="M192" s="12" t="n">
+      <c r="M191" s="3" t="n">
         <v>13.711764</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregando info a capas de poligonos/cambio en coordenas en unos puntos
</commit_message>
<xml_diff>
--- a/puntos_ce.xlsx
+++ b/puntos_ce.xlsx
@@ -2209,8 +2209,8 @@
   </sheetPr>
   <dimension ref="A1:T240"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A163" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O116" activeCellId="0" sqref="O116:O191"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I69" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T88" activeCellId="0" sqref="T88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7955,10 +7955,10 @@
         <v>281</v>
       </c>
       <c r="S88" s="0" t="n">
-        <v>-89.203406</v>
+        <v>-89.202442</v>
       </c>
       <c r="T88" s="0" t="n">
-        <v>13.700315</v>
+        <v>13.701425</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16847,10 +16847,10 @@
         <v>662</v>
       </c>
       <c r="S228" s="0" t="n">
-        <v>-89.200731</v>
+        <v>-89.20075</v>
       </c>
       <c r="T228" s="0" t="n">
-        <v>13.690548</v>
+        <v>13.69069</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17467,10 +17467,10 @@
         <v>688</v>
       </c>
       <c r="S238" s="0" t="n">
-        <v>-89.187345</v>
+        <v>-89.18716</v>
       </c>
       <c r="T238" s="0" t="n">
-        <v>13.692056</v>
+        <v>13.69169</v>
       </c>
     </row>
     <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>